<commit_message>
new results for c2c
</commit_message>
<xml_diff>
--- a/migforecasting/clustering/for paper/examples for improv test.xlsx
+++ b/migforecasting/clustering/for paper/examples for improv test.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="examples" sheetId="1" r:id="rId1"/>
@@ -1635,94 +1635,94 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="30"/>
                 <c:pt idx="0">
-                  <c:v>-140.74899999999994</c:v>
+                  <c:v>-141.35299999999989</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-146.71599999999987</c:v>
+                  <c:v>-142.40799999999984</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-159.93199999999999</c:v>
+                  <c:v>-146.70199999999997</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-187.04899999999998</c:v>
+                  <c:v>-191.87799999999996</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-128.40999999999994</c:v>
+                  <c:v>-129.77099999999993</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-142.56999999999982</c:v>
+                  <c:v>-145.54599999999985</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-126.36899999999989</c:v>
+                  <c:v>-126.19799999999991</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-69.602999999999895</c:v>
+                  <c:v>-68.389999999999915</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-86.481999999999886</c:v>
+                  <c:v>-91.423999999999893</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-44.18499999999996</c:v>
+                  <c:v>-54.461999999999932</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-59.221999999999944</c:v>
+                  <c:v>-65.255999999999929</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>-158.73100000000017</c:v>
+                  <c:v>-160.41000000000011</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>-173.87099999999992</c:v>
+                  <c:v>-174.51399999999992</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>-88.013999999999996</c:v>
+                  <c:v>-63.915000000000006</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>-74.768000000000001</c:v>
+                  <c:v>-74.513000000000005</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.8140000000000065</c:v>
+                  <c:v>-53.878999999999905</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>-59.026999999999987</c:v>
+                  <c:v>-108.63200000000002</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>13.420999999999992</c:v>
+                  <c:v>-113.20799999999983</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>-75.507000000000033</c:v>
+                  <c:v>-205.11800000000017</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>-58.750000000000014</c:v>
+                  <c:v>8.0069999999999908</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>-197.49700000000004</c:v>
+                  <c:v>-214.90500000000006</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>-122.875</c:v>
+                  <c:v>-99.260000000000048</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>-191.58400000000009</c:v>
+                  <c:v>-197.89600000000002</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>-193.36200000000025</c:v>
+                  <c:v>-179.38700000000023</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>-188.84100000000001</c:v>
+                  <c:v>-194.65200000000002</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>-195.10499999999982</c:v>
+                  <c:v>-192.83299999999986</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>-118.74599999999982</c:v>
+                  <c:v>-125.4409999999998</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>-280.59900000000033</c:v>
+                  <c:v>-286.47400000000033</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>-85.670999999999964</c:v>
+                  <c:v>-83.578999999999979</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>-234.333</c:v>
+                  <c:v>-232.68800000000005</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1767,94 +1767,94 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="30"/>
                 <c:pt idx="0">
-                  <c:v>-87.33299999999997</c:v>
+                  <c:v>-80.321999999999989</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-92.926999999999978</c:v>
+                  <c:v>-102.13499999999998</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-107.68599999999999</c:v>
+                  <c:v>-106.40899999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-186.20799999999997</c:v>
+                  <c:v>-194.41</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-76.975999999999971</c:v>
+                  <c:v>-79.969999999999985</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-116.59099999999989</c:v>
+                  <c:v>-124.12199999999993</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-124.21499999999992</c:v>
+                  <c:v>-125.93799999999987</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-56.097999999999971</c:v>
+                  <c:v>-65.623999999999967</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-89.161999999999964</c:v>
+                  <c:v>-93.367999999999967</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-59.36399999999999</c:v>
+                  <c:v>-56.262999999999977</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-33.309000000000005</c:v>
+                  <c:v>-37.85199999999999</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>-101.45999999999998</c:v>
+                  <c:v>-113.64699999999998</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>-165.82299999999995</c:v>
+                  <c:v>-185.47899999999998</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>-76.695000000000007</c:v>
+                  <c:v>-54.69100000000001</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>-51.128999999999984</c:v>
+                  <c:v>-43.817999999999998</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>-33.237999999999992</c:v>
+                  <c:v>-28.80899999999999</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>-187.94099999999997</c:v>
+                  <c:v>-190.02499999999995</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>-143.13800000000001</c:v>
+                  <c:v>-146.08799999999997</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>-79.863000000000028</c:v>
+                  <c:v>-139.21299999999999</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>-96.802999999999969</c:v>
+                  <c:v>-108.69000000000001</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>-74.227999999999994</c:v>
+                  <c:v>-78.413999999999973</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>-122.875</c:v>
+                  <c:v>-99.260000000000048</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>-214.62100000000004</c:v>
+                  <c:v>-215.59</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>-191.50400000000022</c:v>
+                  <c:v>-180.08200000000016</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>-190.46999999999997</c:v>
+                  <c:v>-192.48499999999996</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>-99.288999999999959</c:v>
+                  <c:v>-110.13099999999994</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>-116.65599999999998</c:v>
+                  <c:v>-124.44599999999994</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>-177.57900000000001</c:v>
+                  <c:v>-179.33</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>-105.25399999999999</c:v>
+                  <c:v>-116.44999999999997</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>-176.25199999999995</c:v>
+                  <c:v>-175.52500000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1899,94 +1899,94 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="30"/>
                 <c:pt idx="0">
-                  <c:v>-83.953999999999979</c:v>
+                  <c:v>-88.49799999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-81.792999999999964</c:v>
+                  <c:v>-75.112999999999985</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-142.77299999999997</c:v>
+                  <c:v>-143.61200000000002</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-184.68099999999998</c:v>
+                  <c:v>-178.74099999999996</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-72.106999999999971</c:v>
+                  <c:v>-71.772999999999982</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-127.85399999999997</c:v>
+                  <c:v>-148.29300000000001</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-217.63900000000004</c:v>
+                  <c:v>-204.07999999999996</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-70.777999999999992</c:v>
+                  <c:v>-75.577999999999975</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-82.573999999999984</c:v>
+                  <c:v>-78.123999999999995</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-43.571999999999989</c:v>
+                  <c:v>-43.769999999999996</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-26.684000000000005</c:v>
+                  <c:v>-36.071999999999989</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>-107.75</c:v>
+                  <c:v>-118.97</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>-68.205999999999989</c:v>
+                  <c:v>-73.092000000000013</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>-89.818000000000012</c:v>
+                  <c:v>-69.450000000000017</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>-42.427999999999997</c:v>
+                  <c:v>-47.326000000000001</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>-22.391999999999992</c:v>
+                  <c:v>-4.6049999999999978</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>-171.63199999999995</c:v>
+                  <c:v>-189.67699999999999</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>-150.91599999999997</c:v>
+                  <c:v>-153.63</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>-76.243000000000023</c:v>
+                  <c:v>-143.08799999999999</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>-101.88300000000001</c:v>
+                  <c:v>-68.823999999999998</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>-75.795999999999978</c:v>
+                  <c:v>-80.34899999999999</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>-125.92900000000002</c:v>
+                  <c:v>-96.960000000000065</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>-219.29300000000003</c:v>
+                  <c:v>-222.66199999999998</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>-180.74600000000007</c:v>
+                  <c:v>-160.74700000000007</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>-169.71700000000001</c:v>
+                  <c:v>-168.81299999999999</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>-129.161</c:v>
+                  <c:v>-132.56599999999997</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>-106.78600000000002</c:v>
+                  <c:v>-104.31399999999996</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>-101.53999999999998</c:v>
+                  <c:v>-121.46</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>-118.31599999999996</c:v>
+                  <c:v>-113.16200000000001</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>-150.62599999999995</c:v>
+                  <c:v>-153.83099999999996</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2105,6 +2105,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2173,6 +2174,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -12243,7 +12245,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="F101" sqref="F101"/>
     </sheetView>
   </sheetViews>
@@ -15783,8 +15785,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="S5" sqref="S5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15808,28 +15810,28 @@
     </row>
     <row r="2" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B2" s="11">
-        <v>-140.74899999999994</v>
+        <v>-141.35299999999989</v>
       </c>
       <c r="C2" s="11">
-        <v>-87.33299999999997</v>
+        <v>-80.321999999999989</v>
       </c>
       <c r="D2" s="11">
-        <v>-83.953999999999979</v>
+        <v>-88.49799999999999</v>
       </c>
       <c r="E2" s="11">
         <f>IF(D2&gt;C2,1,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B3" s="11">
-        <v>-146.71599999999987</v>
+        <v>-142.40799999999984</v>
       </c>
       <c r="C3" s="11">
-        <v>-92.926999999999978</v>
+        <v>-102.13499999999998</v>
       </c>
       <c r="D3" s="11">
-        <v>-81.792999999999964</v>
+        <v>-75.112999999999985</v>
       </c>
       <c r="E3" s="11">
         <f t="shared" ref="E3:E31" si="0">IF(D3&gt;C3,1,0)</f>
@@ -15838,13 +15840,13 @@
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" s="11">
-        <v>-159.93199999999999</v>
+        <v>-146.70199999999997</v>
       </c>
       <c r="C4" s="11">
-        <v>-107.68599999999999</v>
+        <v>-106.40899999999999</v>
       </c>
       <c r="D4" s="11">
-        <v>-142.77299999999997</v>
+        <v>-143.61200000000002</v>
       </c>
       <c r="E4" s="11">
         <f t="shared" si="0"/>
@@ -15853,13 +15855,13 @@
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5" s="11">
-        <v>-187.04899999999998</v>
+        <v>-191.87799999999996</v>
       </c>
       <c r="C5" s="11">
-        <v>-186.20799999999997</v>
+        <v>-194.41</v>
       </c>
       <c r="D5" s="11">
-        <v>-184.68099999999998</v>
+        <v>-178.74099999999996</v>
       </c>
       <c r="E5" s="11">
         <f t="shared" si="0"/>
@@ -15868,13 +15870,13 @@
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B6" s="11">
-        <v>-128.40999999999994</v>
+        <v>-129.77099999999993</v>
       </c>
       <c r="C6" s="11">
-        <v>-76.975999999999971</v>
+        <v>-79.969999999999985</v>
       </c>
       <c r="D6" s="11">
-        <v>-72.106999999999971</v>
+        <v>-71.772999999999982</v>
       </c>
       <c r="E6" s="11">
         <f t="shared" si="0"/>
@@ -15883,13 +15885,13 @@
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B7" s="11">
-        <v>-142.56999999999982</v>
+        <v>-145.54599999999985</v>
       </c>
       <c r="C7" s="11">
-        <v>-116.59099999999989</v>
+        <v>-124.12199999999993</v>
       </c>
       <c r="D7" s="11">
-        <v>-127.85399999999997</v>
+        <v>-148.29300000000001</v>
       </c>
       <c r="E7" s="11">
         <f t="shared" si="0"/>
@@ -15898,13 +15900,13 @@
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B8" s="11">
-        <v>-126.36899999999989</v>
+        <v>-126.19799999999991</v>
       </c>
       <c r="C8" s="11">
-        <v>-124.21499999999992</v>
+        <v>-125.93799999999987</v>
       </c>
       <c r="D8" s="11">
-        <v>-217.63900000000004</v>
+        <v>-204.07999999999996</v>
       </c>
       <c r="E8" s="11">
         <f t="shared" si="0"/>
@@ -15913,13 +15915,13 @@
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B9" s="11">
-        <v>-69.602999999999895</v>
+        <v>-68.389999999999915</v>
       </c>
       <c r="C9" s="11">
-        <v>-56.097999999999971</v>
+        <v>-65.623999999999967</v>
       </c>
       <c r="D9" s="11">
-        <v>-70.777999999999992</v>
+        <v>-75.577999999999975</v>
       </c>
       <c r="E9" s="11">
         <f t="shared" si="0"/>
@@ -15928,13 +15930,13 @@
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B10" s="11">
-        <v>-86.481999999999886</v>
+        <v>-91.423999999999893</v>
       </c>
       <c r="C10" s="11">
-        <v>-89.161999999999964</v>
+        <v>-93.367999999999967</v>
       </c>
       <c r="D10" s="11">
-        <v>-82.573999999999984</v>
+        <v>-78.123999999999995</v>
       </c>
       <c r="E10" s="11">
         <f t="shared" si="0"/>
@@ -15943,13 +15945,13 @@
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B11" s="11">
-        <v>-44.18499999999996</v>
+        <v>-54.461999999999932</v>
       </c>
       <c r="C11" s="11">
-        <v>-59.36399999999999</v>
+        <v>-56.262999999999977</v>
       </c>
       <c r="D11" s="11">
-        <v>-43.571999999999989</v>
+        <v>-43.769999999999996</v>
       </c>
       <c r="E11" s="11">
         <f t="shared" si="0"/>
@@ -15958,13 +15960,13 @@
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B12" s="11">
-        <v>-59.221999999999944</v>
+        <v>-65.255999999999929</v>
       </c>
       <c r="C12" s="11">
-        <v>-33.309000000000005</v>
+        <v>-37.85199999999999</v>
       </c>
       <c r="D12" s="11">
-        <v>-26.684000000000005</v>
+        <v>-36.071999999999989</v>
       </c>
       <c r="E12" s="11">
         <f t="shared" si="0"/>
@@ -15973,13 +15975,13 @@
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B13" s="11">
-        <v>-158.73100000000017</v>
+        <v>-160.41000000000011</v>
       </c>
       <c r="C13" s="11">
-        <v>-101.45999999999998</v>
+        <v>-113.64699999999998</v>
       </c>
       <c r="D13" s="11">
-        <v>-107.75</v>
+        <v>-118.97</v>
       </c>
       <c r="E13" s="11">
         <f t="shared" si="0"/>
@@ -15988,13 +15990,13 @@
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B14" s="11">
-        <v>-173.87099999999992</v>
+        <v>-174.51399999999992</v>
       </c>
       <c r="C14" s="11">
-        <v>-165.82299999999995</v>
+        <v>-185.47899999999998</v>
       </c>
       <c r="D14" s="11">
-        <v>-68.205999999999989</v>
+        <v>-73.092000000000013</v>
       </c>
       <c r="E14" s="11">
         <f t="shared" si="0"/>
@@ -16003,13 +16005,13 @@
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B15" s="11">
-        <v>-88.013999999999996</v>
+        <v>-63.915000000000006</v>
       </c>
       <c r="C15" s="11">
-        <v>-76.695000000000007</v>
+        <v>-54.69100000000001</v>
       </c>
       <c r="D15" s="11">
-        <v>-89.818000000000012</v>
+        <v>-69.450000000000017</v>
       </c>
       <c r="E15" s="11">
         <f t="shared" si="0"/>
@@ -16018,28 +16020,28 @@
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B16" s="11">
-        <v>-74.768000000000001</v>
+        <v>-74.513000000000005</v>
       </c>
       <c r="C16" s="11">
-        <v>-51.128999999999984</v>
+        <v>-43.817999999999998</v>
       </c>
       <c r="D16" s="11">
-        <v>-42.427999999999997</v>
+        <v>-47.326000000000001</v>
       </c>
       <c r="E16" s="11">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B17" s="11">
-        <v>0.8140000000000065</v>
+        <v>-53.878999999999905</v>
       </c>
       <c r="C17" s="11">
-        <v>-33.237999999999992</v>
+        <v>-28.80899999999999</v>
       </c>
       <c r="D17" s="11">
-        <v>-22.391999999999992</v>
+        <v>-4.6049999999999978</v>
       </c>
       <c r="E17" s="11">
         <f t="shared" si="0"/>
@@ -16048,13 +16050,13 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B18" s="11">
-        <v>-59.026999999999987</v>
+        <v>-108.63200000000002</v>
       </c>
       <c r="C18" s="11">
-        <v>-187.94099999999997</v>
+        <v>-190.02499999999995</v>
       </c>
       <c r="D18" s="11">
-        <v>-171.63199999999995</v>
+        <v>-189.67699999999999</v>
       </c>
       <c r="E18" s="11">
         <f t="shared" si="0"/>
@@ -16063,13 +16065,13 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B19" s="11">
-        <v>13.420999999999992</v>
+        <v>-113.20799999999983</v>
       </c>
       <c r="C19" s="11">
-        <v>-143.13800000000001</v>
+        <v>-146.08799999999997</v>
       </c>
       <c r="D19" s="11">
-        <v>-150.91599999999997</v>
+        <v>-153.63</v>
       </c>
       <c r="E19" s="11">
         <f t="shared" si="0"/>
@@ -16078,43 +16080,43 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B20" s="11">
-        <v>-75.507000000000033</v>
+        <v>-205.11800000000017</v>
       </c>
       <c r="C20" s="11">
-        <v>-79.863000000000028</v>
+        <v>-139.21299999999999</v>
       </c>
       <c r="D20" s="11">
-        <v>-76.243000000000023</v>
+        <v>-143.08799999999999</v>
       </c>
       <c r="E20" s="11">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B21" s="11">
-        <v>-58.750000000000014</v>
+        <v>8.0069999999999908</v>
       </c>
       <c r="C21" s="11">
-        <v>-96.802999999999969</v>
+        <v>-108.69000000000001</v>
       </c>
       <c r="D21" s="11">
-        <v>-101.88300000000001</v>
+        <v>-68.823999999999998</v>
       </c>
       <c r="E21" s="11">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B22" s="11">
-        <v>-197.49700000000004</v>
+        <v>-214.90500000000006</v>
       </c>
       <c r="C22" s="11">
-        <v>-74.227999999999994</v>
+        <v>-78.413999999999973</v>
       </c>
       <c r="D22" s="11">
-        <v>-75.795999999999978</v>
+        <v>-80.34899999999999</v>
       </c>
       <c r="E22" s="11">
         <f t="shared" si="0"/>
@@ -16123,28 +16125,28 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B23" s="11">
-        <v>-122.875</v>
+        <v>-99.260000000000048</v>
       </c>
       <c r="C23" s="11">
-        <v>-122.875</v>
+        <v>-99.260000000000048</v>
       </c>
       <c r="D23" s="11">
-        <v>-125.92900000000002</v>
+        <v>-96.960000000000065</v>
       </c>
       <c r="E23" s="11">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B24" s="11">
-        <v>-191.58400000000009</v>
+        <v>-197.89600000000002</v>
       </c>
       <c r="C24" s="11">
-        <v>-214.62100000000004</v>
+        <v>-215.59</v>
       </c>
       <c r="D24" s="11">
-        <v>-219.29300000000003</v>
+        <v>-222.66199999999998</v>
       </c>
       <c r="E24" s="11">
         <f t="shared" si="0"/>
@@ -16153,13 +16155,13 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B25" s="11">
-        <v>-193.36200000000025</v>
+        <v>-179.38700000000023</v>
       </c>
       <c r="C25" s="11">
-        <v>-191.50400000000022</v>
+        <v>-180.08200000000016</v>
       </c>
       <c r="D25" s="11">
-        <v>-180.74600000000007</v>
+        <v>-160.74700000000007</v>
       </c>
       <c r="E25" s="11">
         <f t="shared" si="0"/>
@@ -16168,13 +16170,13 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B26" s="11">
-        <v>-188.84100000000001</v>
+        <v>-194.65200000000002</v>
       </c>
       <c r="C26" s="11">
-        <v>-190.46999999999997</v>
+        <v>-192.48499999999996</v>
       </c>
       <c r="D26" s="11">
-        <v>-169.71700000000001</v>
+        <v>-168.81299999999999</v>
       </c>
       <c r="E26" s="11">
         <f t="shared" si="0"/>
@@ -16183,13 +16185,13 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B27" s="11">
-        <v>-195.10499999999982</v>
+        <v>-192.83299999999986</v>
       </c>
       <c r="C27" s="11">
-        <v>-99.288999999999959</v>
+        <v>-110.13099999999994</v>
       </c>
       <c r="D27" s="11">
-        <v>-129.161</v>
+        <v>-132.56599999999997</v>
       </c>
       <c r="E27" s="11">
         <f t="shared" si="0"/>
@@ -16198,13 +16200,13 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B28" s="11">
-        <v>-118.74599999999982</v>
+        <v>-125.4409999999998</v>
       </c>
       <c r="C28" s="11">
-        <v>-116.65599999999998</v>
+        <v>-124.44599999999994</v>
       </c>
       <c r="D28" s="11">
-        <v>-106.78600000000002</v>
+        <v>-104.31399999999996</v>
       </c>
       <c r="E28" s="11">
         <f t="shared" si="0"/>
@@ -16213,13 +16215,13 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B29" s="11">
-        <v>-280.59900000000033</v>
+        <v>-286.47400000000033</v>
       </c>
       <c r="C29" s="11">
-        <v>-177.57900000000001</v>
+        <v>-179.33</v>
       </c>
       <c r="D29" s="11">
-        <v>-101.53999999999998</v>
+        <v>-121.46</v>
       </c>
       <c r="E29" s="11">
         <f t="shared" si="0"/>
@@ -16228,28 +16230,28 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B30" s="11">
-        <v>-85.670999999999964</v>
+        <v>-83.578999999999979</v>
       </c>
       <c r="C30" s="11">
-        <v>-105.25399999999999</v>
+        <v>-116.44999999999997</v>
       </c>
       <c r="D30" s="11">
-        <v>-118.31599999999996</v>
+        <v>-113.16200000000001</v>
       </c>
       <c r="E30" s="11">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B31" s="11">
-        <v>-234.333</v>
+        <v>-232.68800000000005</v>
       </c>
       <c r="C31" s="11">
-        <v>-176.25199999999995</v>
+        <v>-175.52500000000001</v>
       </c>
       <c r="D31" s="11">
-        <v>-150.62599999999995</v>
+        <v>-153.83099999999996</v>
       </c>
       <c r="E31" s="11">
         <f t="shared" si="0"/>
@@ -16262,15 +16264,15 @@
       </c>
       <c r="B32" s="20">
         <f>AVERAGE(B2:B31)</f>
-        <v>-125.81109999999997</v>
+        <v>-135.22283333333331</v>
       </c>
       <c r="C32" s="20">
         <f>AVERAGE(C2:C31)</f>
-        <v>-114.48956666666665</v>
+        <v>-118.28619999999999</v>
       </c>
       <c r="D32" s="20">
         <f>AVERAGE(D2:D31)</f>
-        <v>-111.45289999999997</v>
+        <v>-112.23933333333331</v>
       </c>
     </row>
   </sheetData>

</xml_diff>